<commit_message>
Làm phần báo cáo
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/HoaiBao/Transaction.xlsx
+++ b/QuanLyChiTieu/Data/HoaiBao/Transaction.xlsx
@@ -16,43 +16,88 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
+    <x:t>fsafsasd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>241512413</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nạp tiền</x:t>
+  </x:si>
+  <x:si>
+    <x:t>transt2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fasdafsd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2141254213</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11/10/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ngày giao dịch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>transt1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sfafasdfa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42134124</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rút tiền</x:t>
+  </x:si>
+  <x:si>
+    <x:t>transt0</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ghi chú</x:t>
   </x:si>
   <x:si>
     <x:t>Số tiền</x:t>
   </x:si>
   <x:si>
-    <x:t>Ngày giao dịch</x:t>
-  </x:si>
-  <x:si>
     <x:t>Loại giao dịch</x:t>
   </x:si>
   <x:si>
     <x:t>Mã giao dịch</x:t>
   </x:si>
   <x:si>
-    <x:t>transt0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rút tiền</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11/10/2024 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>42134124</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sfafasdfa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>transt1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2141254213</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fasdafsd</x:t>
+    <x:t>transt3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/4/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5344223</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sfsadfsa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>transt4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>421424</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ỉa chải</x:t>
+  </x:si>
+  <x:si>
+    <x:t>transt5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/2/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>521432</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dfasa</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -411,33 +456,33 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>9</x:v>
@@ -445,19 +490,87 @@
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="D3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>12</x:v>
+      <x:c r="C5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>